<commit_message>
update cleveland columbus and birmingham
</commit_message>
<xml_diff>
--- a/applications/us_states/Birmingham_projections.xlsx
+++ b/applications/us_states/Birmingham_projections.xlsx
@@ -520,76 +520,76 @@
     </row>
     <row r="4" spans="1:24">
       <c r="A4">
-        <v>7749</v>
+        <v>8926</v>
       </c>
       <c r="B4">
-        <v>3555</v>
+        <v>2859</v>
       </c>
       <c r="C4">
-        <v>23390</v>
+        <v>18748</v>
       </c>
       <c r="D4">
-        <v>2.406608695652174</v>
+        <v>2.772265838509316</v>
       </c>
       <c r="E4">
-        <v>1.10416149068323</v>
+        <v>0.8878881987577639</v>
       </c>
       <c r="F4">
-        <v>7.264194732919256</v>
+        <v>5.822628571428573</v>
       </c>
       <c r="G4">
-        <v>88175</v>
+        <v>0.4164993788819875</v>
       </c>
       <c r="H4">
-        <v>52330</v>
+        <v>0.2248447204968944</v>
       </c>
       <c r="I4">
-        <v>125932</v>
+        <v>0.6099037142857143</v>
       </c>
       <c r="J4">
-        <v>0.1357742857142857</v>
+        <v>0.1273685714285715</v>
       </c>
       <c r="K4">
-        <v>0.0996552380952381</v>
+        <v>0.09181428571428571</v>
       </c>
       <c r="L4">
-        <v>0.2287984662857142</v>
+        <v>0.1663270857142857</v>
       </c>
       <c r="M4">
-        <v>8004</v>
+        <v>8148</v>
       </c>
       <c r="N4">
-        <v>1529</v>
+        <v>1506</v>
       </c>
       <c r="O4">
-        <v>25167</v>
+        <v>26457</v>
       </c>
       <c r="P4">
-        <v>2.598900779220779</v>
+        <v>2.645766233766234</v>
       </c>
       <c r="Q4">
-        <v>0.4965584415584415</v>
+        <v>0.489025974025974</v>
       </c>
       <c r="R4">
-        <v>8.171371993506492</v>
+        <v>8.589992837662338</v>
       </c>
       <c r="S4">
-        <v>70102</v>
+        <v>0.3294981818181818</v>
       </c>
       <c r="T4">
-        <v>28418</v>
+        <v>0.1228571428571428</v>
       </c>
       <c r="U4">
-        <v>138896</v>
+        <v>0.6873832597402595</v>
       </c>
       <c r="V4">
-        <v>0.1750270400000001</v>
+        <v>0.1622889142857143</v>
       </c>
       <c r="W4">
-        <v>0.107432380952381</v>
+        <v>0.09775619047619047</v>
       </c>
       <c r="X4">
-        <v>0.3442502472380952</v>
+        <v>0.2961675474285713</v>
       </c>
     </row>
   </sheetData>

</xml_diff>